<commit_message>
Export mit Benefits Advanced
</commit_message>
<xml_diff>
--- a/Documentation/Keyword_Search_mitBenefits_Advanced.xlsx
+++ b/Documentation/Keyword_Search_mitBenefits_Advanced.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16125" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -318,37 +318,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -686,20 +689,20 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="74.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="74.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.875" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="74.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="74.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -720,13 +723,13 @@
       </c>
       <c r="G1" s="1">
         <f>SUM(D:D)</f>
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -737,13 +740,13 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E2" s="2">
         <v>41765</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -760,7 +763,7 @@
         <v>41765</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -777,7 +780,7 @@
         <v>41765</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -791,7 +794,7 @@
         <v>41765</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -811,11 +814,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">

</xml_diff>